<commit_message>
commit my allure extent
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12540" windowHeight="5610"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15705" windowHeight="5490"/>
   </bookViews>
   <sheets>
     <sheet name="addbank" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>